<commit_message>
recursively train and use model
</commit_message>
<xml_diff>
--- a/DRL_Automated_Trading/results14/BAS.DE.xlsx
+++ b/DRL_Automated_Trading/results14/BAS.DE.xlsx
@@ -3052,28 +3052,28 @@
         <v>44223</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D82" t="n">
-        <v>11447.20846951242</v>
+        <v>1104895.051640702</v>
       </c>
       <c r="E82" t="n">
-        <v>17947</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>1105621.506219352</v>
+        <v>1104895.051640702</v>
       </c>
       <c r="G82" t="n">
         <v>60.96697485651305</v>
       </c>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>726.454578649904</v>
       </c>
       <c r="I82" t="n">
-        <v>1114842.588154802</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>-21394.74498361209</v>
       </c>
     </row>
     <row r="83">
@@ -3087,13 +3087,13 @@
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>11447.20846951242</v>
+        <v>1104895.051640702</v>
       </c>
       <c r="E83" t="n">
-        <v>17947</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>1101088.122236685</v>
+        <v>1104895.051640702</v>
       </c>
       <c r="G83" t="n">
         <v>60.71437642877208</v>
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>1114842.588154802</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -3119,22 +3119,22 @@
         <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>137.4814393792352</v>
+        <v>11230.30572204882</v>
       </c>
       <c r="E84" t="n">
-        <v>18132</v>
+        <v>17952</v>
       </c>
       <c r="F84" t="n">
-        <v>1104035.127232308</v>
+        <v>1104169.338221203</v>
       </c>
       <c r="G84" t="n">
         <v>60.88118496541632</v>
       </c>
       <c r="H84" t="n">
-        <v>46.70781153116121</v>
+        <v>725.7134194994924</v>
       </c>
       <c r="I84" t="n">
-        <v>1126152.315184935</v>
+        <v>1093664.745918653</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
@@ -3151,22 +3151,22 @@
         <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>1.162059759233451</v>
+        <v>91.25608974918651</v>
       </c>
       <c r="E85" t="n">
-        <v>18134</v>
+        <v>18132</v>
       </c>
       <c r="F85" t="n">
-        <v>1117503.287074315</v>
+        <v>1117470.131724685</v>
       </c>
       <c r="G85" t="n">
         <v>61.62468981000085</v>
       </c>
       <c r="H85" t="n">
-        <v>13.07</v>
+        <v>46.60546649948009</v>
       </c>
       <c r="I85" t="n">
-        <v>1126288.634564555</v>
+        <v>1104803.795550953</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
@@ -3183,13 +3183,13 @@
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>1.162059759233451</v>
+        <v>91.25608974918651</v>
       </c>
       <c r="E86" t="n">
-        <v>18134</v>
+        <v>18132</v>
       </c>
       <c r="F86" t="n">
-        <v>1132109.392454032</v>
+        <v>1132074.626196122</v>
       </c>
       <c r="G86" t="n">
         <v>62.43014395027424</v>
@@ -3198,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="n">
-        <v>1126288.634564555</v>
+        <v>1104803.795550953</v>
       </c>
       <c r="J86" t="n">
         <v>0</v>
@@ -3215,22 +3215,22 @@
         <v>1</v>
       </c>
       <c r="D87" t="n">
-        <v>1.162059759233451</v>
+        <v>15.28410675375371</v>
       </c>
       <c r="E87" t="n">
-        <v>18134</v>
+        <v>18133</v>
       </c>
       <c r="F87" t="n">
-        <v>1140665.721698938</v>
+        <v>1140616.941762937</v>
       </c>
       <c r="G87" t="n">
         <v>62.9019829954328</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>13.07</v>
       </c>
       <c r="I87" t="n">
-        <v>1126288.634564555</v>
+        <v>1104879.767533949</v>
       </c>
       <c r="J87" t="n">
         <v>0</v>
@@ -3247,13 +3247,13 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>1.162059759233451</v>
+        <v>15.28410675375371</v>
       </c>
       <c r="E88" t="n">
-        <v>18134</v>
+        <v>18133</v>
       </c>
       <c r="F88" t="n">
-        <v>1146283.463569858</v>
+        <v>1146234.373843305</v>
       </c>
       <c r="G88" t="n">
         <v>63.21177354748533</v>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="n">
-        <v>1126288.634564555</v>
+        <v>1104879.767533949</v>
       </c>
       <c r="J88" t="n">
         <v>0</v>
@@ -3279,13 +3279,13 @@
         <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>1.162059759233451</v>
+        <v>15.28410675375371</v>
       </c>
       <c r="E89" t="n">
-        <v>18134</v>
+        <v>18133</v>
       </c>
       <c r="F89" t="n">
-        <v>1150518.305039218</v>
+        <v>1150468.981782199</v>
       </c>
       <c r="G89" t="n">
         <v>63.44530401342554</v>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="n">
-        <v>1126288.634564555</v>
+        <v>1104879.767533949</v>
       </c>
       <c r="J89" t="n">
         <v>0</v>
@@ -3311,13 +3311,13 @@
         <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>1.162059759233451</v>
+        <v>15.28410675375371</v>
       </c>
       <c r="E90" t="n">
-        <v>18134</v>
+        <v>18133</v>
       </c>
       <c r="F90" t="n">
-        <v>1166853.01246516</v>
+        <v>1166802.788430187</v>
       </c>
       <c r="G90" t="n">
         <v>64.34608196787256</v>
@@ -3326,7 +3326,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="n">
-        <v>1126288.634564555</v>
+        <v>1104879.767533949</v>
       </c>
       <c r="J90" t="n">
         <v>0</v>
@@ -3343,13 +3343,13 @@
         <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>1.162059759233451</v>
+        <v>15.28410675375371</v>
       </c>
       <c r="E91" t="n">
-        <v>18134</v>
+        <v>18133</v>
       </c>
       <c r="F91" t="n">
-        <v>1157864.583022393</v>
+        <v>1157814.854654644</v>
       </c>
       <c r="G91" t="n">
         <v>63.85041474372086</v>
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="n">
-        <v>1126288.634564555</v>
+        <v>1104879.767533949</v>
       </c>
       <c r="J91" t="n">
         <v>0</v>
@@ -3375,25 +3375,25 @@
         <v>-1</v>
       </c>
       <c r="D92" t="n">
-        <v>1160641.330943952</v>
+        <v>1160591.445594956</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>1160641.330943952</v>
+        <v>1160591.445594956</v>
       </c>
       <c r="G92" t="n">
         <v>64.04582348417503</v>
       </c>
       <c r="H92" t="n">
-        <v>766.7941778372181</v>
+        <v>766.7557503431276</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
       </c>
       <c r="J92" t="n">
-        <v>34351.53431963781</v>
+        <v>55696.39395425399</v>
       </c>
     </row>
     <row r="93">
@@ -3407,22 +3407,22 @@
         <v>1</v>
       </c>
       <c r="D93" t="n">
-        <v>11755.96304077184</v>
+        <v>11770.09995091012</v>
       </c>
       <c r="E93" t="n">
-        <v>17944</v>
+        <v>17943</v>
       </c>
       <c r="F93" t="n">
-        <v>1159882.505018765</v>
+        <v>1159832.658060091</v>
       </c>
       <c r="G93" t="n">
         <v>63.98386881286188</v>
       </c>
       <c r="H93" t="n">
-        <v>758.8259251867961</v>
+        <v>758.7875348655084</v>
       </c>
       <c r="I93" t="n">
-        <v>1148885.36790318</v>
+        <v>1148821.345644046</v>
       </c>
       <c r="J93" t="n">
         <v>0</v>
@@ -3439,13 +3439,13 @@
         <v>1</v>
       </c>
       <c r="D94" t="n">
-        <v>109.0276686962747</v>
+        <v>123.1645788345572</v>
       </c>
       <c r="E94" t="n">
-        <v>18127</v>
+        <v>18126</v>
       </c>
       <c r="F94" t="n">
-        <v>1149145.419165021</v>
+        <v>1149096.167958455</v>
       </c>
       <c r="G94" t="n">
         <v>63.38811670416091</v>
@@ -3454,7 +3454,7 @@
         <v>46.91001521411687</v>
       </c>
       <c r="I94" t="n">
-        <v>1160532.303275256</v>
+        <v>1160468.281016122</v>
       </c>
       <c r="J94" t="n">
         <v>0</v>
@@ -3471,13 +3471,13 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>109.0276686962747</v>
+        <v>123.1645788345572</v>
       </c>
       <c r="E95" t="n">
-        <v>18127</v>
+        <v>18126</v>
       </c>
       <c r="F95" t="n">
-        <v>1163400.390616195</v>
+        <v>1163350.35301522</v>
       </c>
       <c r="G95" t="n">
         <v>64.17451111311847</v>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="I95" t="n">
-        <v>1160532.303275256</v>
+        <v>1160468.281016122</v>
       </c>
       <c r="J95" t="n">
         <v>0</v>
@@ -3503,25 +3503,25 @@
         <v>-1</v>
       </c>
       <c r="D96" t="n">
-        <v>1166431.468671797</v>
+        <v>1166381.259998495</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>1166431.468671797</v>
+        <v>1166381.259998495</v>
       </c>
       <c r="G96" t="n">
         <v>64.3842139676204</v>
       </c>
       <c r="H96" t="n">
-        <v>770.205587954633</v>
+        <v>770.1669574262525</v>
       </c>
       <c r="I96" t="n">
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>5790.137727844529</v>
+        <v>5789.814403539058</v>
       </c>
     </row>
     <row r="97">
@@ -3535,13 +3535,13 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>1166431.468671797</v>
+        <v>1166381.259998495</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>1166431.468671797</v>
+        <v>1166381.259998495</v>
       </c>
       <c r="G97" t="n">
         <v>64.34608796993739</v>
@@ -3567,22 +3567,22 @@
         <v>1</v>
       </c>
       <c r="D98" t="n">
-        <v>11834.76731110389</v>
+        <v>11848.72396606154</v>
       </c>
       <c r="E98" t="n">
-        <v>17993</v>
+        <v>17992</v>
       </c>
       <c r="F98" t="n">
-        <v>1165669.218001382</v>
+        <v>1165619.047804193</v>
       </c>
       <c r="G98" t="n">
         <v>64.12685214751728</v>
       </c>
       <c r="H98" t="n">
-        <v>762.2506704141672</v>
+        <v>762.2121943028786</v>
       </c>
       <c r="I98" t="n">
-        <v>1154596.701360693</v>
+        <v>1154532.536032434</v>
       </c>
       <c r="J98" t="n">
         <v>0</v>
@@ -3599,13 +3599,13 @@
         <v>1</v>
       </c>
       <c r="D99" t="n">
-        <v>120.4713432589714</v>
+        <v>134.4279982166216</v>
       </c>
       <c r="E99" t="n">
-        <v>18174</v>
+        <v>18173</v>
       </c>
       <c r="F99" t="n">
-        <v>1171625.10237466</v>
+        <v>1171574.598556908</v>
       </c>
       <c r="G99" t="n">
         <v>64.46047270999236</v>
@@ -3614,7 +3614,7 @@
         <v>46.95040733630518</v>
       </c>
       <c r="I99" t="n">
-        <v>1166310.997328538</v>
+        <v>1166246.832000279</v>
       </c>
       <c r="J99" t="n">
         <v>0</v>
@@ -3631,25 +3631,25 @@
         <v>-1</v>
       </c>
       <c r="D100" t="n">
-        <v>1179681.953496544</v>
+        <v>1179631.002512448</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>1179681.953496544</v>
+        <v>1179631.002512448</v>
       </c>
       <c r="G100" t="n">
         <v>64.94660701743402</v>
       </c>
       <c r="H100" t="n">
-        <v>778.1537815609075</v>
+        <v>778.1148135966971</v>
       </c>
       <c r="I100" t="n">
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>13250.48482474708</v>
+        <v>13249.74251395278</v>
       </c>
     </row>
     <row r="101">
@@ -3663,13 +3663,13 @@
         <v>-1</v>
       </c>
       <c r="D101" t="n">
-        <v>1179681.953496544</v>
+        <v>1179631.002512448</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>1179681.953496544</v>
+        <v>1179631.002512448</v>
       </c>
       <c r="G101" t="n">
         <v>65.29452483735329</v>
@@ -3695,22 +3695,22 @@
         <v>1</v>
       </c>
       <c r="D102" t="n">
-        <v>11966.20093134848</v>
+        <v>11980.77440306496</v>
       </c>
       <c r="E102" t="n">
-        <v>17820</v>
+        <v>17819</v>
       </c>
       <c r="F102" t="n">
-        <v>1178911.836115433</v>
+        <v>1178860.924422437</v>
       </c>
       <c r="G102" t="n">
         <v>65.4851647129116</v>
       </c>
       <c r="H102" t="n">
-        <v>770.1173811104509</v>
+        <v>770.078090011623</v>
       </c>
       <c r="I102" t="n">
-        <v>1167715.752565195</v>
+        <v>1167650.228109383</v>
       </c>
       <c r="J102" t="n">
         <v>0</v>
@@ -3727,13 +3727,13 @@
         <v>1</v>
       </c>
       <c r="D103" t="n">
-        <v>98.37152936570399</v>
+        <v>112.9450010821909</v>
       </c>
       <c r="E103" t="n">
-        <v>18000</v>
+        <v>17999</v>
       </c>
       <c r="F103" t="n">
-        <v>1182177.064511853</v>
+        <v>1182125.966945071</v>
       </c>
       <c r="G103" t="n">
         <v>65.67103849902709</v>
@@ -3742,7 +3742,7 @@
         <v>47.04247215789493</v>
       </c>
       <c r="I103" t="n">
-        <v>1179583.581967178</v>
+        <v>1179518.057511366</v>
       </c>
       <c r="J103" t="n">
         <v>0</v>
@@ -3759,25 +3759,25 @@
         <v>-1</v>
       </c>
       <c r="D104" t="n">
-        <v>1150618.411087706</v>
+        <v>1150569.062893337</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>1150618.411087706</v>
+        <v>1150569.062893337</v>
       </c>
       <c r="G104" t="n">
         <v>63.9600421118416</v>
       </c>
       <c r="H104" t="n">
-        <v>760.7184548078893</v>
+        <v>760.6800787826222</v>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>-29063.54240883724</v>
+        <v>-29061.9396191116</v>
       </c>
     </row>
     <row r="105">
@@ -3791,22 +3791,22 @@
         <v>1</v>
       </c>
       <c r="D105" t="n">
-        <v>11664.89056678071</v>
+        <v>11681.17651086884</v>
       </c>
       <c r="E105" t="n">
-        <v>17352</v>
+        <v>17351</v>
       </c>
       <c r="F105" t="n">
-        <v>1149865.540697628</v>
+        <v>1149816.231860127</v>
       </c>
       <c r="G105" t="n">
         <v>65.59478158891466</v>
       </c>
       <c r="H105" t="n">
-        <v>752.8703900785083</v>
+        <v>752.831033209555</v>
       </c>
       <c r="I105" t="n">
-        <v>1138953.520520926</v>
+        <v>1138887.886382468</v>
       </c>
       <c r="J105" t="n">
         <v>0</v>
@@ -3823,13 +3823,13 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>11664.89056678071</v>
+        <v>11681.17651086884</v>
       </c>
       <c r="E106" t="n">
-        <v>17352</v>
+        <v>17351</v>
       </c>
       <c r="F106" t="n">
-        <v>1157639.442044858</v>
+        <v>1157589.685195523</v>
       </c>
       <c r="G106" t="n">
         <v>66.04279342312569</v>
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="I106" t="n">
-        <v>1138953.520520926</v>
+        <v>1138887.886382468</v>
       </c>
       <c r="J106" t="n">
         <v>0</v>
@@ -3855,13 +3855,13 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>11664.89056678071</v>
+        <v>11681.17651086884</v>
       </c>
       <c r="E107" t="n">
-        <v>17352</v>
+        <v>17351</v>
       </c>
       <c r="F107" t="n">
-        <v>1187245.968098869</v>
+        <v>1187194.505018204</v>
       </c>
       <c r="G107" t="n">
         <v>67.74902475403923</v>
@@ -3870,7 +3870,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="n">
-        <v>1138953.520520926</v>
+        <v>1138887.886382468</v>
       </c>
       <c r="J107" t="n">
         <v>0</v>
@@ -3887,22 +3887,22 @@
         <v>1</v>
       </c>
       <c r="D108" t="n">
-        <v>138.7994308262401</v>
+        <v>87.51983882052519</v>
       </c>
       <c r="E108" t="n">
         <v>17522</v>
       </c>
       <c r="F108" t="n">
-        <v>1183312.218815632</v>
+        <v>1183260.939223626</v>
       </c>
       <c r="G108" t="n">
         <v>67.52502108120109</v>
       </c>
       <c r="H108" t="n">
-        <v>46.83755215028251</v>
+        <v>46.87806716293124</v>
       </c>
       <c r="I108" t="n">
-        <v>1150479.61165688</v>
+        <v>1150481.543054516</v>
       </c>
       <c r="J108" t="n">
         <v>0</v>
@@ -3919,22 +3919,22 @@
         <v>1</v>
       </c>
       <c r="D109" t="n">
-        <v>138.7994308262401</v>
+        <v>6.653150175272721</v>
       </c>
       <c r="E109" t="n">
-        <v>17522</v>
+        <v>17523</v>
       </c>
       <c r="F109" t="n">
-        <v>1188072.37787294</v>
+        <v>1188008.028280934</v>
       </c>
       <c r="G109" t="n">
         <v>67.79668864525247</v>
       </c>
       <c r="H109" t="n">
-        <v>0</v>
+        <v>13.07</v>
       </c>
       <c r="I109" t="n">
-        <v>1150479.61165688</v>
+        <v>1150562.409743161</v>
       </c>
       <c r="J109" t="n">
         <v>0</v>
@@ -3951,13 +3951,13 @@
         <v>1</v>
       </c>
       <c r="D110" t="n">
-        <v>138.7994308262401</v>
+        <v>6.653150175272721</v>
       </c>
       <c r="E110" t="n">
-        <v>17522</v>
+        <v>17523</v>
       </c>
       <c r="F110" t="n">
-        <v>1199930.787040246</v>
+        <v>1199867.114220821</v>
       </c>
       <c r="G110" t="n">
         <v>68.47346122642504</v>
@@ -3966,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="I110" t="n">
-        <v>1150479.61165688</v>
+        <v>1150562.409743161</v>
       </c>
       <c r="J110" t="n">
         <v>0</v>
@@ -3983,22 +3983,22 @@
         <v>1</v>
       </c>
       <c r="D111" t="n">
-        <v>56.92711170530185</v>
+        <v>6.653150175272721</v>
       </c>
       <c r="E111" t="n">
         <v>17523</v>
       </c>
       <c r="F111" t="n">
-        <v>1205679.965067907</v>
+        <v>1205629.691106377</v>
       </c>
       <c r="G111" t="n">
         <v>68.80231912093828</v>
       </c>
       <c r="H111" t="n">
-        <v>13.07</v>
+        <v>0</v>
       </c>
       <c r="I111" t="n">
-        <v>1150561.483976001</v>
+        <v>1150562.409743161</v>
       </c>
       <c r="J111" t="n">
         <v>0</v>
@@ -4015,13 +4015,13 @@
         <v>-1</v>
       </c>
       <c r="D112" t="n">
-        <v>1201881.92025782</v>
+        <v>1201831.64629629</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>1201881.92025782</v>
+        <v>1201831.64629629</v>
       </c>
       <c r="G112" t="n">
         <v>68.63074319773708</v>
@@ -4033,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>51263.50917011313</v>
+        <v>51262.58340295288</v>
       </c>
     </row>
     <row r="113">
@@ -4047,13 +4047,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="n">
-        <v>12216.63267221217</v>
+        <v>12166.35871068211</v>
       </c>
       <c r="E113" t="n">
         <v>17251</v>
       </c>
       <c r="F113" t="n">
-        <v>1201098.641052791</v>
+        <v>1201048.367091261</v>
       </c>
       <c r="G113" t="n">
         <v>68.91670096693403</v>
@@ -4079,22 +4079,22 @@
         <v>1</v>
       </c>
       <c r="D114" t="n">
-        <v>114.0305373320759</v>
+        <v>132.6860165727535</v>
       </c>
       <c r="E114" t="n">
-        <v>17426</v>
+        <v>17425</v>
       </c>
       <c r="F114" t="n">
-        <v>1200558.198907285</v>
+        <v>1200507.966278619</v>
       </c>
       <c r="G114" t="n">
         <v>68.8881079059998</v>
       </c>
       <c r="H114" t="n">
-        <v>47.18325133012998</v>
+        <v>47.14191846538638</v>
       </c>
       <c r="I114" t="n">
-        <v>1201767.889720488</v>
+        <v>1201698.960279717</v>
       </c>
       <c r="J114" t="n">
         <v>0</v>
@@ -4111,13 +4111,13 @@
         <v>1</v>
       </c>
       <c r="D115" t="n">
-        <v>32.86359082287674</v>
+        <v>51.51907006355443</v>
       </c>
       <c r="E115" t="n">
-        <v>17427</v>
+        <v>17426</v>
       </c>
       <c r="F115" t="n">
-        <v>1186758.350406636</v>
+        <v>1186708.908939367</v>
       </c>
       <c r="G115" t="n">
         <v>68.09694650919911</v>
@@ -4126,7 +4126,7 @@
         <v>13.07</v>
       </c>
       <c r="I115" t="n">
-        <v>1201849.056666997</v>
+        <v>1201780.127226226</v>
       </c>
       <c r="J115" t="n">
         <v>0</v>
@@ -4143,13 +4143,13 @@
         <v>1</v>
       </c>
       <c r="D116" t="n">
-        <v>32.86359082287674</v>
+        <v>51.51907006355443</v>
       </c>
       <c r="E116" t="n">
-        <v>17427</v>
+        <v>17426</v>
       </c>
       <c r="F116" t="n">
-        <v>1172140.306879275</v>
+        <v>1172091.70422784</v>
       </c>
       <c r="G116" t="n">
         <v>67.25813067587377</v>
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="I116" t="n">
-        <v>1201849.056666997</v>
+        <v>1201780.127226226</v>
       </c>
       <c r="J116" t="n">
         <v>0</v>
@@ -4175,25 +4175,25 @@
         <v>-1</v>
       </c>
       <c r="D117" t="n">
-        <v>1170038.874445779</v>
+        <v>1169990.388365322</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>1170038.874445779</v>
+        <v>1169990.388365322</v>
       </c>
       <c r="G117" t="n">
         <v>67.1818688191716</v>
       </c>
       <c r="H117" t="n">
-        <v>772.4170567470222</v>
+        <v>772.3767476257306</v>
       </c>
       <c r="I117" t="n">
         <v>0</v>
       </c>
       <c r="J117" t="n">
-        <v>-31843.04581204033</v>
+        <v>-31841.25793096749</v>
       </c>
     </row>
     <row r="118">
@@ -4207,22 +4207,22 @@
         <v>1</v>
       </c>
       <c r="D118" t="n">
-        <v>11874.93976436859</v>
+        <v>11894.75363582691</v>
       </c>
       <c r="E118" t="n">
-        <v>16956</v>
+        <v>16955</v>
       </c>
       <c r="F118" t="n">
-        <v>1169274.484718807</v>
+        <v>1169226.039593747</v>
       </c>
       <c r="G118" t="n">
         <v>68.25899651771869</v>
       </c>
       <c r="H118" t="n">
-        <v>764.3897269726629</v>
+        <v>764.3487715747523</v>
       </c>
       <c r="I118" t="n">
-        <v>1158163.934681411</v>
+        <v>1158095.634729495</v>
       </c>
       <c r="J118" t="n">
         <v>0</v>
@@ -4239,25 +4239,25 @@
         <v>-1</v>
       </c>
       <c r="D119" t="n">
-        <v>1157929.915476645</v>
+        <v>1157882.135285488</v>
       </c>
       <c r="E119" t="n">
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>1157929.915476645</v>
+        <v>1157882.135285488</v>
       </c>
       <c r="G119" t="n">
         <v>67.63464340176864</v>
       </c>
       <c r="H119" t="n">
-        <v>758.0378081122335</v>
+        <v>757.9972273261925</v>
       </c>
       <c r="I119" t="n">
         <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>-12108.95896913391</v>
+        <v>-12108.25307983393</v>
       </c>
     </row>
     <row r="120">
@@ -4271,22 +4271,22 @@
         <v>1</v>
       </c>
       <c r="D120" t="n">
-        <v>11740.16653486778</v>
+        <v>11758.85504399138</v>
       </c>
       <c r="E120" t="n">
-        <v>17243</v>
+        <v>17242</v>
       </c>
       <c r="F120" t="n">
-        <v>1157172.705952995</v>
+        <v>1157124.965619143</v>
       </c>
       <c r="G120" t="n">
         <v>66.42884297501169</v>
       </c>
       <c r="H120" t="n">
-        <v>757.209523650876</v>
+        <v>757.1696663450909</v>
       </c>
       <c r="I120" t="n">
-        <v>1146189.748941778</v>
+        <v>1146123.280241497</v>
       </c>
       <c r="J120" t="n">
         <v>0</v>
@@ -4303,25 +4303,25 @@
         <v>-1</v>
       </c>
       <c r="D121" t="n">
-        <v>1147298.908077111</v>
+        <v>1147251.736312991</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>1147298.908077111</v>
+        <v>1147251.736312991</v>
       </c>
       <c r="G121" t="n">
         <v>65.89981313164419</v>
       </c>
       <c r="H121" t="n">
-        <v>751.7362866973646</v>
+        <v>751.6967468094855</v>
       </c>
       <c r="I121" t="n">
         <v>0</v>
       </c>
       <c r="J121" t="n">
-        <v>-10631.00739953411</v>
+        <v>-10630.39897249686</v>
       </c>
     </row>
     <row r="122">
@@ -4332,25 +4332,25 @@
         <v>44279</v>
       </c>
       <c r="C122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122" t="n">
-        <v>1147298.908077111</v>
+        <v>11673.87117744583</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>17218</v>
       </c>
       <c r="F122" t="n">
-        <v>1147298.908077111</v>
+        <v>1146500.890101637</v>
       </c>
       <c r="G122" t="n">
         <v>65.90934016286391</v>
       </c>
       <c r="H122" t="n">
-        <v>0</v>
+        <v>750.8462113545145</v>
       </c>
       <c r="I122" t="n">
-        <v>0</v>
+        <v>1135577.865135545</v>
       </c>
       <c r="J122" t="n">
         <v>0</v>
@@ -4367,13 +4367,13 @@
         <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>1147298.908077111</v>
+        <v>11673.87117744583</v>
       </c>
       <c r="E123" t="n">
-        <v>0</v>
+        <v>17218</v>
       </c>
       <c r="F123" t="n">
-        <v>1147298.908077111</v>
+        <v>1154214.628752711</v>
       </c>
       <c r="G123" t="n">
         <v>66.35734449850536</v>
@@ -4382,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="n">
-        <v>0</v>
+        <v>1135577.865135545</v>
       </c>
       <c r="J123" t="n">
         <v>0</v>
@@ -4399,13 +4399,13 @@
         <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>1147298.908077111</v>
+        <v>11673.87117744583</v>
       </c>
       <c r="E124" t="n">
-        <v>0</v>
+        <v>17218</v>
       </c>
       <c r="F124" t="n">
-        <v>1147298.908077111</v>
+        <v>1166523.970812716</v>
       </c>
       <c r="G124" t="n">
         <v>67.07225575765304</v>
@@ -4414,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="I124" t="n">
-        <v>0</v>
+        <v>1135577.865135545</v>
       </c>
       <c r="J124" t="n">
         <v>0</v>
@@ -4431,13 +4431,13 @@
         <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>1147298.908077111</v>
+        <v>11673.87117744583</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>17218</v>
       </c>
       <c r="F125" t="n">
-        <v>1147298.908077111</v>
+        <v>1160533.466173487</v>
       </c>
       <c r="G125" t="n">
         <v>66.72433470763393</v>
@@ -4446,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>1135577.865135545</v>
       </c>
       <c r="J125" t="n">
         <v>0</v>
@@ -4463,22 +4463,22 @@
         <v>1</v>
       </c>
       <c r="D126" t="n">
-        <v>11659.88093626001</v>
+        <v>108.0543726249646</v>
       </c>
       <c r="E126" t="n">
-        <v>16749</v>
+        <v>17388</v>
       </c>
       <c r="F126" t="n">
-        <v>1146548.025190559</v>
+        <v>1178293.919337324</v>
       </c>
       <c r="G126" t="n">
         <v>67.758561362129</v>
       </c>
       <c r="H126" t="n">
-        <v>750.8828865525793</v>
+        <v>46.86137325893716</v>
       </c>
       <c r="I126" t="n">
-        <v>1135639.027140851</v>
+        <v>1147143.681940366</v>
       </c>
       <c r="J126" t="n">
         <v>0</v>
@@ -4495,25 +4495,25 @@
         <v>-1</v>
       </c>
       <c r="D127" t="n">
-        <v>1153057.005526386</v>
+        <v>1185053.895940665</v>
       </c>
       <c r="E127" t="n">
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>1153057.005526386</v>
+        <v>1185053.895940665</v>
       </c>
       <c r="G127" t="n">
         <v>68.19227213623091</v>
       </c>
       <c r="H127" t="n">
-        <v>755.2414196058389</v>
+        <v>781.38633674287</v>
       </c>
       <c r="I127" t="n">
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>5758.097449274501</v>
+        <v>37802.15962767391</v>
       </c>
     </row>
     <row r="128">
@@ -4527,22 +4527,22 @@
         <v>1</v>
       </c>
       <c r="D128" t="n">
-        <v>11731.59263626132</v>
+        <v>12049.60255811765</v>
       </c>
       <c r="E128" t="n">
-        <v>16788</v>
+        <v>17254</v>
       </c>
       <c r="F128" t="n">
-        <v>1152302.712854255</v>
+        <v>1184280.607337797</v>
       </c>
       <c r="G128" t="n">
         <v>67.93966644138632</v>
       </c>
       <c r="H128" t="n">
-        <v>754.2926721307963</v>
+        <v>773.2886028678079</v>
       </c>
       <c r="I128" t="n">
-        <v>1141325.412890124</v>
+        <v>1173004.293382548</v>
       </c>
       <c r="J128" t="n">
         <v>0</v>
@@ -4559,25 +4559,25 @@
         <v>-1</v>
       </c>
       <c r="D129" t="n">
-        <v>1168660.825276586</v>
+        <v>1201094.728640805</v>
       </c>
       <c r="E129" t="n">
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>1168660.825276586</v>
+        <v>1201094.728640805</v>
       </c>
       <c r="G129" t="n">
         <v>68.95960203238479</v>
       </c>
       <c r="H129" t="n">
-        <v>764.5662793518056</v>
+        <v>783.8473840800604</v>
       </c>
       <c r="I129" t="n">
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>15603.81975019979</v>
+        <v>16040.83270013961</v>
       </c>
     </row>
     <row r="130">
@@ -4591,13 +4591,13 @@
         <v>-1</v>
       </c>
       <c r="D130" t="n">
-        <v>1168660.825276586</v>
+        <v>1201094.728640805</v>
       </c>
       <c r="E130" t="n">
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>1168660.825276586</v>
+        <v>1201094.728640805</v>
       </c>
       <c r="G130" t="n">
         <v>69.07398324573191</v>
@@ -4623,22 +4623,22 @@
         <v>1</v>
       </c>
       <c r="D131" t="n">
-        <v>11865.52157224854</v>
+        <v>12210.06716921047</v>
       </c>
       <c r="E131" t="n">
-        <v>16870</v>
+        <v>17338</v>
       </c>
       <c r="F131" t="n">
-        <v>1167897.256235787</v>
+        <v>1200311.917530588</v>
       </c>
       <c r="G131" t="n">
         <v>68.52588824324475</v>
       </c>
       <c r="H131" t="n">
-        <v>763.5690407981234</v>
+        <v>782.8111102168265</v>
       </c>
       <c r="I131" t="n">
-        <v>1156795.303704337</v>
+        <v>1188884.661471594</v>
       </c>
       <c r="J131" t="n">
         <v>0</v>
@@ -4655,22 +4655,22 @@
         <v>1</v>
       </c>
       <c r="D132" t="n">
-        <v>117.3523270737153</v>
+        <v>121.5427134201044</v>
       </c>
       <c r="E132" t="n">
-        <v>17042</v>
+        <v>17515</v>
       </c>
       <c r="F132" t="n">
-        <v>1159488.429542775</v>
+        <v>1191670.915875784</v>
       </c>
       <c r="G132" t="n">
         <v>68.0302239887162</v>
       </c>
       <c r="H132" t="n">
-        <v>46.97071911563552</v>
+        <v>47.17480978760166</v>
       </c>
       <c r="I132" t="n">
-        <v>1168543.472949512</v>
+        <v>1200973.185927385</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
@@ -4687,13 +4687,13 @@
         <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>36.47610871524783</v>
+        <v>40.66649506163693</v>
       </c>
       <c r="E133" t="n">
-        <v>17043</v>
+        <v>17516</v>
       </c>
       <c r="F133" t="n">
-        <v>1155657.855592077</v>
+        <v>1187734.387261979</v>
       </c>
       <c r="G133" t="n">
         <v>67.80621835846752</v>
@@ -4702,7 +4702,7 @@
         <v>13.07</v>
       </c>
       <c r="I133" t="n">
-        <v>1168624.34916787</v>
+        <v>1201054.062145743</v>
       </c>
       <c r="J133" t="n">
         <v>0</v>
@@ -4719,25 +4719,25 @@
         <v>-1</v>
       </c>
       <c r="D134" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="E134" t="n">
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="G134" t="n">
         <v>68.15413602414809</v>
       </c>
       <c r="H134" t="n">
-        <v>766.8805641557335</v>
+        <v>786.2227079593868</v>
       </c>
       <c r="I134" t="n">
         <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>-7840.289472470293</v>
+        <v>-8052.438254724722</v>
       </c>
     </row>
     <row r="135">
@@ -4751,13 +4751,13 @@
         <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="E135" t="n">
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="G135" t="n">
         <v>67.65848009485364</v>
@@ -4783,13 +4783,13 @@
         <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="E136" t="n">
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="G136" t="n">
         <v>68.03975481951089</v>
@@ -4815,13 +4815,13 @@
         <v>-1</v>
       </c>
       <c r="D137" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="E137" t="n">
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>1160820.535804115</v>
+        <v>1193042.29038608</v>
       </c>
       <c r="G137" t="n">
         <v>68.56878850008975</v>
@@ -4847,22 +4847,22 @@
         <v>1</v>
       </c>
       <c r="D138" t="n">
-        <v>11749.74959999679</v>
+        <v>12137.11819537688</v>
       </c>
       <c r="E138" t="n">
-        <v>16675</v>
+        <v>17137</v>
       </c>
       <c r="F138" t="n">
-        <v>1160061.598694658</v>
+        <v>1192264.264098538</v>
       </c>
       <c r="G138" t="n">
         <v>68.86427880627656</v>
       </c>
       <c r="H138" t="n">
-        <v>758.9371094567971</v>
+        <v>778.026287541897</v>
       </c>
       <c r="I138" t="n">
-        <v>1149070.786204119</v>
+        <v>1180905.172190703</v>
       </c>
       <c r="J138" t="n">
         <v>0</v>
@@ -4879,13 +4879,13 @@
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>11749.74959999679</v>
+        <v>12137.11819537688</v>
       </c>
       <c r="E139" t="n">
-        <v>16675</v>
+        <v>17137</v>
       </c>
       <c r="F139" t="n">
-        <v>1146074.250840876</v>
+        <v>1177889.380730007</v>
       </c>
       <c r="G139" t="n">
         <v>68.0254573457799</v>
@@ -4894,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="I139" t="n">
-        <v>1149070.786204119</v>
+        <v>1180905.172190703</v>
       </c>
       <c r="J139" t="n">
         <v>0</v>
@@ -4911,13 +4911,13 @@
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>11749.74959999679</v>
+        <v>12137.11819537688</v>
       </c>
       <c r="E140" t="n">
-        <v>16675</v>
+        <v>17137</v>
       </c>
       <c r="F140" t="n">
-        <v>1139557.436109524</v>
+        <v>1171192.010172214</v>
       </c>
       <c r="G140" t="n">
         <v>67.63464386863728</v>
@@ -4926,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="n">
-        <v>1149070.786204119</v>
+        <v>1180905.172190703</v>
       </c>
       <c r="J140" t="n">
         <v>0</v>
@@ -4943,25 +4943,25 @@
         <v>-1</v>
       </c>
       <c r="D141" t="n">
-        <v>1136110.351728956</v>
+        <v>1167651.358410308</v>
       </c>
       <c r="E141" t="n">
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>1136110.351728956</v>
+        <v>1167651.358410308</v>
       </c>
       <c r="G141" t="n">
         <v>67.4726006295807</v>
       </c>
       <c r="H141" t="n">
-        <v>745.0133692989548</v>
+        <v>763.7167741934746</v>
       </c>
       <c r="I141" t="n">
         <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>-24710.18407515949</v>
+        <v>-25390.9319757726</v>
       </c>
     </row>
     <row r="142">
@@ -4975,13 +4975,13 @@
         <v>-1</v>
       </c>
       <c r="D142" t="n">
-        <v>1136110.351728956</v>
+        <v>1167651.358410308</v>
       </c>
       <c r="E142" t="n">
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>1136110.351728956</v>
+        <v>1167651.358410308</v>
       </c>
       <c r="G142" t="n">
         <v>66.66237829668425</v>
@@ -5007,22 +5007,22 @@
         <v>1</v>
       </c>
       <c r="D143" t="n">
-        <v>11511.68028408802</v>
+        <v>11849.69433275563</v>
       </c>
       <c r="E143" t="n">
-        <v>16578</v>
+        <v>17038</v>
       </c>
       <c r="F143" t="n">
-        <v>1135366.089083676</v>
+        <v>1166888.38519579</v>
       </c>
       <c r="G143" t="n">
         <v>67.79191752923079</v>
       </c>
       <c r="H143" t="n">
-        <v>744.2626452797527</v>
+        <v>762.9732145178207</v>
       </c>
       <c r="I143" t="n">
-        <v>1124598.671444868</v>
+        <v>1155801.664077552</v>
       </c>
       <c r="J143" t="n">
         <v>0</v>
@@ -5039,13 +5039,13 @@
         <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>11511.68028408802</v>
+        <v>11849.69433275563</v>
       </c>
       <c r="E144" t="n">
-        <v>16578</v>
+        <v>17038</v>
       </c>
       <c r="F144" t="n">
-        <v>1136709.401875027</v>
+        <v>1168268.971716422</v>
       </c>
       <c r="G144" t="n">
         <v>67.87294737549396</v>
@@ -5054,7 +5054,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="n">
-        <v>1124598.671444868</v>
+        <v>1155801.664077552</v>
       </c>
       <c r="J144" t="n">
         <v>0</v>
@@ -5071,22 +5071,22 @@
         <v>1</v>
       </c>
       <c r="D145" t="n">
-        <v>112.6268867310731</v>
+        <v>110.548019310155</v>
       </c>
       <c r="E145" t="n">
-        <v>16745</v>
+        <v>17210</v>
       </c>
       <c r="F145" t="n">
-        <v>1138400.829945387</v>
+        <v>1170008.426468965</v>
       </c>
       <c r="G145" t="n">
         <v>67.97779653978237</v>
       </c>
       <c r="H145" t="n">
-        <v>46.7613752132862</v>
+        <v>46.96530860290554</v>
       </c>
       <c r="I145" t="n">
-        <v>1135997.724842225</v>
+        <v>1167540.810390997</v>
       </c>
       <c r="J145" t="n">
         <v>0</v>
@@ -5103,13 +5103,13 @@
         <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>112.6268867310731</v>
+        <v>110.548019310155</v>
       </c>
       <c r="E146" t="n">
-        <v>16745</v>
+        <v>17210</v>
       </c>
       <c r="F146" t="n">
-        <v>1128823.951129285</v>
+        <v>1160165.602675288</v>
       </c>
       <c r="G146" t="n">
         <v>67.40587185682614</v>
@@ -5118,7 +5118,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="n">
-        <v>1135997.724842225</v>
+        <v>1167540.810390997</v>
       </c>
       <c r="J146" t="n">
         <v>0</v>
@@ -5135,13 +5135,13 @@
         <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>112.6268867310731</v>
+        <v>110.548019310155</v>
       </c>
       <c r="E147" t="n">
-        <v>16745</v>
+        <v>17210</v>
       </c>
       <c r="F147" t="n">
-        <v>1139526.185102826</v>
+        <v>1171165.032157799</v>
       </c>
       <c r="G147" t="n">
         <v>68.04500198364258</v>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="I147" t="n">
-        <v>1135997.724842225</v>
+        <v>1167540.810390997</v>
       </c>
       <c r="J147" t="n">
         <v>0</v>
@@ -5167,13 +5167,13 @@
         <v>1</v>
       </c>
       <c r="D148" t="n">
-        <v>32.53188520519422</v>
+        <v>30.45301778427605</v>
       </c>
       <c r="E148" t="n">
-        <v>16746</v>
+        <v>17211</v>
       </c>
       <c r="F148" t="n">
-        <v>1122433.207437573</v>
+        <v>1153597.754279686</v>
       </c>
       <c r="G148" t="n">
         <v>67.02500152587891</v>
@@ -5182,7 +5182,7 @@
         <v>13.07</v>
       </c>
       <c r="I148" t="n">
-        <v>1136077.819843751</v>
+        <v>1167620.905392523</v>
       </c>
       <c r="J148" t="n">
         <v>0</v>
@@ -5199,13 +5199,13 @@
         <v>1</v>
       </c>
       <c r="D149" t="n">
-        <v>32.53188520519422</v>
+        <v>30.45301778427605</v>
       </c>
       <c r="E149" t="n">
-        <v>16746</v>
+        <v>17211</v>
       </c>
       <c r="F149" t="n">
-        <v>1133904.240434705</v>
+        <v>1165387.312915398</v>
       </c>
       <c r="G149" t="n">
         <v>67.71000289916992</v>
@@ -5214,7 +5214,7 @@
         <v>0</v>
       </c>
       <c r="I149" t="n">
-        <v>1136077.819843751</v>
+        <v>1167620.905392523</v>
       </c>
       <c r="J149" t="n">
         <v>0</v>
@@ -5231,25 +5231,25 @@
         <v>-1</v>
       </c>
       <c r="D150" t="n">
-        <v>1144869.083015502</v>
+        <v>1176658.56768717</v>
       </c>
       <c r="E150" t="n">
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>1144869.083015502</v>
+        <v>1176658.56768717</v>
       </c>
       <c r="G150" t="n">
         <v>68.40999984741211</v>
       </c>
       <c r="H150" t="n">
-        <v>757.306314466858</v>
+        <v>776.392704424286</v>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>8758.73128654575</v>
+        <v>9007.20927686221</v>
       </c>
     </row>
     <row r="151">
@@ -5263,22 +5263,22 @@
         <v>1</v>
       </c>
       <c r="D151" t="n">
-        <v>11650.49692068972</v>
+        <v>11934.52355162301</v>
       </c>
       <c r="E151" t="n">
-        <v>16221</v>
+        <v>16672</v>
       </c>
       <c r="F151" t="n">
-        <v>1144119.65152274</v>
+        <v>1175890.244254748</v>
       </c>
       <c r="G151" t="n">
         <v>69.81500244140625</v>
       </c>
       <c r="H151" t="n">
-        <v>749.4314927612305</v>
+        <v>768.3234324218751</v>
       </c>
       <c r="I151" t="n">
-        <v>1133218.586094812</v>
+        <v>1164724.044135547</v>
       </c>
       <c r="J151" t="n">
         <v>0</v>
@@ -5295,13 +5295,13 @@
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>11650.49692068972</v>
+        <v>11934.52355162301</v>
       </c>
       <c r="E152" t="n">
-        <v>16221</v>
+        <v>16672</v>
       </c>
       <c r="F152" t="n">
-        <v>1152473.394744023</v>
+        <v>1184476.250480334</v>
       </c>
       <c r="G152" t="n">
         <v>70.32999801635742</v>
@@ -5310,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="I152" t="n">
-        <v>1133218.586094812</v>
+        <v>1164724.044135547</v>
       </c>
       <c r="J152" t="n">
         <v>0</v>
@@ -5327,25 +5327,25 @@
         <v>-1</v>
       </c>
       <c r="D153" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="E153" t="n">
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="G153" t="n">
         <v>70.67500305175781</v>
       </c>
       <c r="H153" t="n">
-        <v>757.8015347015381</v>
+        <v>776.9261905273438</v>
       </c>
       <c r="I153" t="n">
         <v>0</v>
       </c>
       <c r="J153" t="n">
-        <v>12442.83687304985</v>
+        <v>12792.68055283208</v>
       </c>
     </row>
     <row r="154">
@@ -5359,13 +5359,13 @@
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="E154" t="n">
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="G154" t="n">
         <v>69.39500045776367</v>
@@ -5391,13 +5391,13 @@
         <v>-1</v>
       </c>
       <c r="D155" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="E155" t="n">
         <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="G155" t="n">
         <v>68.91500091552734</v>
@@ -5423,13 +5423,13 @@
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="E156" t="n">
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="G156" t="n">
         <v>68.19000244140625</v>
@@ -5455,13 +5455,13 @@
         <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="E157" t="n">
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>1157311.919888552</v>
+        <v>1189451.248240002</v>
       </c>
       <c r="G157" t="n">
         <v>69.12000274658203</v>
@@ -5487,22 +5487,22 @@
         <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>11734.96792881647</v>
+        <v>12050.81392119703</v>
       </c>
       <c r="E158" t="n">
-        <v>16558</v>
+        <v>17018</v>
       </c>
       <c r="F158" t="n">
-        <v>1156555.077822615</v>
+        <v>1188675.323534234</v>
       </c>
       <c r="G158" t="n">
         <v>69.13999938964844</v>
       </c>
       <c r="H158" t="n">
-        <v>756.8420659362794</v>
+        <v>775.9247057678223</v>
       </c>
       <c r="I158" t="n">
-        <v>1145576.951959735</v>
+        <v>1177400.434318805</v>
       </c>
       <c r="J158" t="n">
         <v>0</v>
@@ -5519,13 +5519,13 @@
         <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>11734.96792881647</v>
+        <v>12050.81392119703</v>
       </c>
       <c r="E159" t="n">
-        <v>16558</v>
+        <v>17018</v>
       </c>
       <c r="F159" t="n">
-        <v>1158542.083300521</v>
+        <v>1190717.530275567</v>
       </c>
       <c r="G159" t="n">
         <v>69.26000213623047</v>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="I159" t="n">
-        <v>1145576.951959735</v>
+        <v>1177400.434318805</v>
       </c>
       <c r="J159" t="n">
         <v>0</v>
@@ -5551,13 +5551,13 @@
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>11734.96792881647</v>
+        <v>12050.81392119703</v>
       </c>
       <c r="E160" t="n">
-        <v>16558</v>
+        <v>17018</v>
       </c>
       <c r="F160" t="n">
-        <v>1130145.047610213</v>
+        <v>1161531.592760308</v>
       </c>
       <c r="G160" t="n">
         <v>67.54499816894531</v>
@@ -5566,7 +5566,7 @@
         <v>0</v>
       </c>
       <c r="I160" t="n">
-        <v>1145576.951959735</v>
+        <v>1177400.434318805</v>
       </c>
       <c r="J160" t="n">
         <v>0</v>
@@ -5583,13 +5583,13 @@
         <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>11734.96792881647</v>
+        <v>12050.81392119703</v>
       </c>
       <c r="E161" t="n">
-        <v>16558</v>
+        <v>17018</v>
       </c>
       <c r="F161" t="n">
-        <v>1121286.520136763</v>
+        <v>1152426.965357049</v>
       </c>
       <c r="G161" t="n">
         <v>67.0099983215332</v>
@@ -5598,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="I161" t="n">
-        <v>1145576.951959735</v>
+        <v>1177400.434318805</v>
       </c>
       <c r="J161" t="n">
         <v>0</v>
@@ -5615,22 +5615,22 @@
         <v>1</v>
       </c>
       <c r="D162" t="n">
-        <v>122.4938650065046</v>
+        <v>99.96196078443612</v>
       </c>
       <c r="E162" t="n">
-        <v>16729</v>
+        <v>17194</v>
       </c>
       <c r="F162" t="n">
-        <v>1131588.380785936</v>
+        <v>1163016.123101226</v>
       </c>
       <c r="G162" t="n">
         <v>67.6349983215332</v>
       </c>
       <c r="H162" t="n">
-        <v>46.88935082778931</v>
+        <v>47.09225582275391</v>
       </c>
       <c r="I162" t="n">
-        <v>1157189.426023545</v>
+        <v>1189351.286279218</v>
       </c>
       <c r="J162" t="n">
         <v>0</v>
@@ -5647,13 +5647,13 @@
         <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>122.4938650065046</v>
+        <v>99.96196078443612</v>
       </c>
       <c r="E163" t="n">
-        <v>16729</v>
+        <v>17194</v>
       </c>
       <c r="F163" t="n">
-        <v>1132926.731417649</v>
+        <v>1164391.674584381</v>
       </c>
       <c r="G163" t="n">
         <v>67.71500015258789</v>
@@ -5662,7 +5662,7 @@
         <v>0</v>
       </c>
       <c r="I163" t="n">
-        <v>1157189.426023545</v>
+        <v>1189351.286279218</v>
       </c>
       <c r="J163" t="n">
         <v>0</v>
@@ -5679,25 +5679,25 @@
         <v>-1</v>
       </c>
       <c r="D164" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="G164" t="n">
         <v>66.77499771118164</v>
       </c>
       <c r="H164" t="n">
-        <v>740.1973620262147</v>
+        <v>758.8275863876343</v>
       </c>
       <c r="I164" t="n">
         <v>0</v>
       </c>
       <c r="J164" t="n">
-        <v>-40850.68667521351</v>
+        <v>-41980.80321954819</v>
       </c>
     </row>
     <row r="165">
@@ -5711,13 +5711,13 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="G165" t="n">
         <v>66.875</v>
@@ -5743,13 +5743,13 @@
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>1116461.233213338</v>
+        <v>1147470.445020454</v>
       </c>
       <c r="G166" t="n">
         <v>67.15000152587891</v>
@@ -5772,25 +5772,25 @@
         <v>44347</v>
       </c>
       <c r="C167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D167" t="n">
-        <v>1116461.233213338</v>
+        <v>11624.47231225675</v>
       </c>
       <c r="E167" t="n">
-        <v>0</v>
+        <v>16981</v>
       </c>
       <c r="F167" t="n">
-        <v>1116461.233213338</v>
+        <v>1146719.438041016</v>
       </c>
       <c r="G167" t="n">
         <v>66.84500122070312</v>
       </c>
       <c r="H167" t="n">
-        <v>0</v>
+        <v>751.0069794372559</v>
       </c>
       <c r="I167" t="n">
-        <v>0</v>
+        <v>1135845.972708197</v>
       </c>
       <c r="J167" t="n">
         <v>0</v>
@@ -5807,13 +5807,13 @@
         <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>1116461.233213338</v>
+        <v>11624.47231225675</v>
       </c>
       <c r="E168" t="n">
-        <v>0</v>
+        <v>16981</v>
       </c>
       <c r="F168" t="n">
-        <v>1116461.233213338</v>
+        <v>1160728.711219117</v>
       </c>
       <c r="G168" t="n">
         <v>67.66999816894531</v>
@@ -5822,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="I168" t="n">
-        <v>0</v>
+        <v>1135845.972708197</v>
       </c>
       <c r="J168" t="n">
         <v>0</v>
@@ -5839,22 +5839,22 @@
         <v>1</v>
       </c>
       <c r="D169" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E169" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F169" t="n">
-        <v>1115728.650860051</v>
+        <v>1168493.138168824</v>
       </c>
       <c r="G169" t="n">
         <v>68.12999725341797</v>
       </c>
       <c r="H169" t="n">
-        <v>732.5823532867432</v>
+        <v>46.81750372314453</v>
       </c>
       <c r="I169" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J169" t="n">
         <v>0</v>
@@ -5871,13 +5871,13 @@
         <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E170" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F170" t="n">
-        <v>1111757.280010442</v>
+        <v>1164291.716904176</v>
       </c>
       <c r="G170" t="n">
         <v>67.88500213623047</v>
@@ -5886,7 +5886,7 @@
         <v>0</v>
       </c>
       <c r="I170" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J170" t="n">
         <v>0</v>
@@ -5903,13 +5903,13 @@
         <v>0</v>
       </c>
       <c r="D171" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E171" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F171" t="n">
-        <v>1121726.395382146</v>
+        <v>1174838.315269959</v>
       </c>
       <c r="G171" t="n">
         <v>68.5</v>
@@ -5918,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="I171" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J171" t="n">
         <v>0</v>
@@ -5935,13 +5935,13 @@
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E172" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F172" t="n">
-        <v>1125940.968174199</v>
+        <v>1179297.026485932</v>
       </c>
       <c r="G172" t="n">
         <v>68.7599983215332</v>
@@ -5950,7 +5950,7 @@
         <v>0</v>
       </c>
       <c r="I172" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J172" t="n">
         <v>0</v>
@@ -5967,13 +5967,13 @@
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E173" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F173" t="n">
-        <v>1114756.090435247</v>
+        <v>1167464.2400365</v>
       </c>
       <c r="G173" t="n">
         <v>68.06999969482422</v>
@@ -5982,7 +5982,7 @@
         <v>0</v>
       </c>
       <c r="I173" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J173" t="n">
         <v>0</v>
@@ -5999,13 +5999,13 @@
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>11341.39538214605</v>
+        <v>131.8152699593869</v>
       </c>
       <c r="E174" t="n">
-        <v>16210</v>
+        <v>17149</v>
       </c>
       <c r="F174" t="n">
-        <v>1110784.657749395</v>
+        <v>1163262.753353608</v>
       </c>
       <c r="G174" t="n">
         <v>67.82500076293945</v>
@@ -6014,7 +6014,7 @@
         <v>0</v>
       </c>
       <c r="I174" t="n">
-        <v>1105119.837831192</v>
+        <v>1147338.629750494</v>
       </c>
       <c r="J174" t="n">
         <v>0</v>
@@ -6031,25 +6031,25 @@
         <v>-1</v>
       </c>
       <c r="D175" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="E175" t="n">
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="G175" t="n">
         <v>67.15499877929688</v>
       </c>
       <c r="H175" t="n">
-        <v>723.0995181274415</v>
+        <v>760.9346444396972</v>
       </c>
       <c r="I175" t="n">
         <v>0</v>
       </c>
       <c r="J175" t="n">
-        <v>-17260.40713691711</v>
+        <v>3541.509671228006</v>
       </c>
     </row>
     <row r="176">
@@ -6063,13 +6063,13 @@
         <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="E176" t="n">
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="G176" t="n">
         <v>67.29500198364258</v>
@@ -6095,13 +6095,13 @@
         <v>-1</v>
       </c>
       <c r="D177" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="G177" t="n">
         <v>67.59000015258789</v>
@@ -6127,13 +6127,13 @@
         <v>0</v>
       </c>
       <c r="D178" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="E178" t="n">
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>1099200.826076421</v>
+        <v>1151011.954691682</v>
       </c>
       <c r="G178" t="n">
         <v>67.22500228881836</v>
@@ -6159,22 +6159,22 @@
         <v>1</v>
       </c>
       <c r="D179" t="n">
-        <v>11157.41094605139</v>
+        <v>11700.6771720544</v>
       </c>
       <c r="E179" t="n">
-        <v>16298</v>
+        <v>17066</v>
       </c>
       <c r="F179" t="n">
-        <v>1098478.483432929</v>
+        <v>1150258.869776119</v>
       </c>
       <c r="G179" t="n">
         <v>66.71500015258789</v>
       </c>
       <c r="H179" t="n">
-        <v>722.3426434921265</v>
+        <v>753.0849155624389</v>
       </c>
       <c r="I179" t="n">
-        <v>1088043.41513037</v>
+        <v>1139311.277519627</v>
       </c>
       <c r="J179" t="n">
         <v>0</v>
@@ -6191,25 +6191,25 @@
         <v>-1</v>
       </c>
       <c r="D180" t="n">
-        <v>1089123.403436519</v>
+        <v>1140466.252668577</v>
       </c>
       <c r="E180" t="n">
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>1089123.403436519</v>
+        <v>1140466.252668577</v>
       </c>
       <c r="G180" t="n">
         <v>66.18500137329102</v>
       </c>
       <c r="H180" t="n">
-        <v>717.1598914291382</v>
+        <v>747.6579400619507</v>
       </c>
       <c r="I180" t="n">
         <v>0</v>
       </c>
       <c r="J180" t="n">
-        <v>-10077.42263990175</v>
+        <v>-10545.702023105</v>
       </c>
     </row>
     <row r="181">
@@ -6223,13 +6223,13 @@
         <v>-1</v>
       </c>
       <c r="D181" t="n">
-        <v>1089123.403436519</v>
+        <v>1140466.252668577</v>
       </c>
       <c r="E181" t="n">
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>1089123.403436519</v>
+        <v>1140466.252668577</v>
       </c>
       <c r="G181" t="n">
         <v>65.19999694824219</v>
@@ -6255,22 +6255,22 @@
         <v>1</v>
       </c>
       <c r="D182" t="n">
-        <v>11025.58203559757</v>
+        <v>11568.24931610715</v>
       </c>
       <c r="E182" t="n">
-        <v>16616</v>
+        <v>17399</v>
       </c>
       <c r="F182" t="n">
-        <v>1088407.024570998</v>
+        <v>1139719.411970984</v>
       </c>
       <c r="G182" t="n">
         <v>64.84000015258789</v>
       </c>
       <c r="H182" t="n">
-        <v>716.3788655212402</v>
+        <v>746.8406975929261</v>
       </c>
       <c r="I182" t="n">
-        <v>1078097.821400922</v>
+        <v>1128898.00335247</v>
       </c>
       <c r="J182" t="n">
         <v>0</v>
@@ -6287,25 +6287,25 @@
         <v>-1</v>
       </c>
       <c r="D183" t="n">
-        <v>1104628.804315114</v>
+        <v>1156708.911045242</v>
       </c>
       <c r="E183" t="n">
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>1104628.804315114</v>
+        <v>1156708.911045242</v>
       </c>
       <c r="G183" t="n">
         <v>65.86000061035156</v>
       </c>
       <c r="H183" t="n">
-        <v>726.547862084961</v>
+        <v>757.4888903717041</v>
       </c>
       <c r="I183" t="n">
         <v>0</v>
       </c>
       <c r="J183" t="n">
-        <v>15505.40087859496</v>
+        <v>16242.65837666555</v>
       </c>
     </row>
     <row r="184">
@@ -6319,22 +6319,22 @@
         <v>1</v>
       </c>
       <c r="D184" t="n">
-        <v>11205.44038039126</v>
+        <v>11763.86168135684</v>
       </c>
       <c r="E184" t="n">
-        <v>16595</v>
+        <v>17377</v>
       </c>
       <c r="F184" t="n">
-        <v>1103903.23563796</v>
+        <v>1155952.447893515</v>
       </c>
       <c r="G184" t="n">
         <v>65.84500122070312</v>
       </c>
       <c r="H184" t="n">
-        <v>725.5686771545411</v>
+        <v>756.463151727295</v>
       </c>
       <c r="I184" t="n">
-        <v>1093423.363934723</v>
+        <v>1144945.049363886</v>
       </c>
       <c r="J184" t="n">
         <v>0</v>
@@ -6351,25 +6351,25 @@
         <v>-1</v>
       </c>
       <c r="D185" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E185" t="n">
         <v>0</v>
       </c>
       <c r="F185" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G185" t="n">
         <v>65.72500228881836</v>
       </c>
       <c r="H185" t="n">
-        <v>724.3738477897645</v>
+        <v>755.2120188636779</v>
       </c>
       <c r="I185" t="n">
         <v>0</v>
       </c>
       <c r="J185" t="n">
-        <v>-3441.324799572118</v>
+        <v>-3596.896609952673</v>
       </c>
     </row>
     <row r="186">
@@ -6383,13 +6383,13 @@
         <v>0</v>
       </c>
       <c r="D186" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E186" t="n">
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G186" t="n">
         <v>65.92999649047852</v>
@@ -6415,13 +6415,13 @@
         <v>0</v>
       </c>
       <c r="D187" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E187" t="n">
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G187" t="n">
         <v>65.63999938964844</v>
@@ -6447,13 +6447,13 @@
         <v>0</v>
       </c>
       <c r="D188" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E188" t="n">
         <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G188" t="n">
         <v>66.28499984741211</v>
@@ -6479,13 +6479,13 @@
         <v>-1</v>
       </c>
       <c r="D189" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E189" t="n">
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G189" t="n">
         <v>66.40500259399414</v>
@@ -6511,13 +6511,13 @@
         <v>0</v>
       </c>
       <c r="D190" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E190" t="n">
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G190" t="n">
         <v>67.15999984741211</v>
@@ -6543,13 +6543,13 @@
         <v>0</v>
       </c>
       <c r="D191" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E191" t="n">
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G191" t="n">
         <v>67.61000061035156</v>
@@ -6575,13 +6575,13 @@
         <v>-1</v>
       </c>
       <c r="D192" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E192" t="n">
         <v>0</v>
       </c>
       <c r="F192" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G192" t="n">
         <v>67.36000061035156</v>
@@ -6607,13 +6607,13 @@
         <v>-1</v>
       </c>
       <c r="D193" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E193" t="n">
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G193" t="n">
         <v>66.63500213623047</v>
@@ -6639,13 +6639,13 @@
         <v>0</v>
       </c>
       <c r="D194" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="E194" t="n">
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>1101187.479515542</v>
+        <v>1153112.01443529</v>
       </c>
       <c r="G194" t="n">
         <v>66.41500091552734</v>
@@ -6671,22 +6671,22 @@
         <v>1</v>
       </c>
       <c r="D195" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E195" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F195" t="n">
-        <v>1100463.955587356</v>
+        <v>1152357.654136529</v>
       </c>
       <c r="G195" t="n">
         <v>65.47000122070312</v>
       </c>
       <c r="H195" t="n">
-        <v>723.5239281860352</v>
+        <v>754.3602987609864</v>
       </c>
       <c r="I195" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J195" t="n">
         <v>0</v>
@@ -6703,13 +6703,13 @@
         <v>0</v>
       </c>
       <c r="D196" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E196" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F196" t="n">
-        <v>1130578.694967239</v>
+        <v>1183893.241599908</v>
       </c>
       <c r="G196" t="n">
         <v>67.27999877929688</v>
@@ -6718,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="I196" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J196" t="n">
         <v>0</v>
@@ -6735,13 +6735,13 @@
         <v>0</v>
       </c>
       <c r="D197" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E197" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F197" t="n">
-        <v>1142142.099889724</v>
+        <v>1196002.22128283</v>
       </c>
       <c r="G197" t="n">
         <v>67.97499847412109</v>
@@ -6750,7 +6750,7 @@
         <v>0</v>
       </c>
       <c r="I197" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J197" t="n">
         <v>0</v>
@@ -6767,13 +6767,13 @@
         <v>0</v>
       </c>
       <c r="D198" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E198" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F198" t="n">
-        <v>1145386.50481221</v>
+        <v>1199399.700965752</v>
       </c>
       <c r="G198" t="n">
         <v>68.16999816894531</v>
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="I198" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J198" t="n">
         <v>0</v>
@@ -6799,13 +6799,13 @@
         <v>0</v>
       </c>
       <c r="D199" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E199" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F199" t="n">
-        <v>1141726.187971084</v>
+        <v>1195566.686160912</v>
       </c>
       <c r="G199" t="n">
         <v>67.95000076293945</v>
@@ -6814,7 +6814,7 @@
         <v>0</v>
       </c>
       <c r="I199" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J199" t="n">
         <v>0</v>
@@ -6831,13 +6831,13 @@
         <v>0</v>
       </c>
       <c r="D200" t="n">
-        <v>11174.07527729741</v>
+        <v>11673.82286821813</v>
       </c>
       <c r="E200" t="n">
-        <v>16638</v>
+        <v>17423</v>
       </c>
       <c r="F200" t="n">
-        <v>1137150.776052444</v>
+        <v>1190775.401038995</v>
       </c>
       <c r="G200" t="n">
         <v>67.67500305175781</v>
@@ -6846,7 +6846,7 @@
         <v>0</v>
       </c>
       <c r="I200" t="n">
-        <v>1090013.404238245</v>
+        <v>1141438.191567071</v>
       </c>
       <c r="J200" t="n">
         <v>0</v>
@@ -6863,25 +6863,25 @@
         <v>-1</v>
       </c>
       <c r="D201" t="n">
-        <v>1128839.46175917</v>
+        <v>1182075.249687768</v>
       </c>
       <c r="E201" t="n">
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>1128839.46175917</v>
+        <v>1182075.249687768</v>
       </c>
       <c r="G201" t="n">
         <v>67.22000122070312</v>
       </c>
       <c r="H201" t="n">
-        <v>740.9938281860352</v>
+        <v>772.6544487609864</v>
       </c>
       <c r="I201" t="n">
         <v>0</v>
       </c>
       <c r="J201" t="n">
-        <v>27651.98224362801</v>
+        <v>28963.23525247816</v>
       </c>
     </row>
     <row r="202">
@@ -6895,22 +6895,22 @@
         <v>1</v>
       </c>
       <c r="D202" t="n">
-        <v>11433.94937965803</v>
+        <v>11986.19552295764</v>
       </c>
       <c r="E202" t="n">
-        <v>17094</v>
+        <v>17900</v>
       </c>
       <c r="F202" t="n">
-        <v>1128099.512421345</v>
+        <v>1181303.709179574</v>
       </c>
       <c r="G202" t="n">
         <v>65.32500076293945</v>
       </c>
       <c r="H202" t="n">
-        <v>739.9493378250122</v>
+        <v>771.5405081939698</v>
       </c>
       <c r="I202" t="n">
-        <v>1117405.512379512</v>
+        <v>1170089.05416481</v>
       </c>
       <c r="J202" t="n">
         <v>0</v>
@@ -6927,22 +6927,22 @@
         <v>1</v>
       </c>
       <c r="D203" t="n">
-        <v>103.3042887934652</v>
+        <v>133.4373643074322</v>
       </c>
       <c r="E203" t="n">
-        <v>17267</v>
+        <v>18081</v>
       </c>
       <c r="F203" t="n">
-        <v>1126343.352941442</v>
+        <v>1179466.634774891</v>
       </c>
       <c r="G203" t="n">
         <v>65.22499847412109</v>
       </c>
       <c r="H203" t="n">
-        <v>46.72035484161377</v>
+        <v>47.03343483428955</v>
       </c>
       <c r="I203" t="n">
-        <v>1128736.157470376</v>
+        <v>1181941.81232346</v>
       </c>
       <c r="J203" t="n">
         <v>0</v>
@@ -6959,13 +6959,13 @@
         <v>0</v>
       </c>
       <c r="D204" t="n">
-        <v>103.3042887934652</v>
+        <v>133.4373643074322</v>
       </c>
       <c r="E204" t="n">
-        <v>17267</v>
+        <v>18081</v>
       </c>
       <c r="F204" t="n">
-        <v>1143610.352941442</v>
+        <v>1197547.634774891</v>
       </c>
       <c r="G204" t="n">
         <v>66.22499847412109</v>
@@ -6974,7 +6974,7 @@
         <v>0</v>
       </c>
       <c r="I204" t="n">
-        <v>1128736.157470376</v>
+        <v>1181941.81232346</v>
       </c>
       <c r="J204" t="n">
         <v>0</v>
@@ -6991,25 +6991,25 @@
         <v>-1</v>
       </c>
       <c r="D205" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E205" t="n">
         <v>0</v>
       </c>
       <c r="F205" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G205" t="n">
         <v>66.94499969482422</v>
       </c>
       <c r="H205" t="n">
-        <v>763.5135858383179</v>
+        <v>796.2095236892701</v>
       </c>
       <c r="I205" t="n">
         <v>0</v>
       </c>
       <c r="J205" t="n">
-        <v>26439.63867431507</v>
+        <v>27694.51763496711</v>
       </c>
     </row>
     <row r="206">
@@ -7023,13 +7023,13 @@
         <v>-1</v>
       </c>
       <c r="D206" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E206" t="n">
         <v>0</v>
       </c>
       <c r="F206" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G206" t="n">
         <v>67.08500289916992</v>
@@ -7055,13 +7055,13 @@
         <v>-1</v>
       </c>
       <c r="D207" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E207" t="n">
         <v>0</v>
       </c>
       <c r="F207" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G207" t="n">
         <v>67.08000183105469</v>
@@ -7087,13 +7087,13 @@
         <v>-1</v>
       </c>
       <c r="D208" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E208" t="n">
         <v>0</v>
       </c>
       <c r="F208" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G208" t="n">
         <v>67.03499984741211</v>
@@ -7119,13 +7119,13 @@
         <v>0</v>
       </c>
       <c r="D209" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E209" t="n">
         <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G209" t="n">
         <v>66.61000061035156</v>
@@ -7151,13 +7151,13 @@
         <v>-1</v>
       </c>
       <c r="D210" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E210" t="n">
         <v>0</v>
       </c>
       <c r="F210" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G210" t="n">
         <v>66.97000122070312</v>
@@ -7183,13 +7183,13 @@
         <v>0</v>
       </c>
       <c r="D211" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="E211" t="n">
         <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>1155279.100433485</v>
+        <v>1209769.767322735</v>
       </c>
       <c r="G211" t="n">
         <v>66.33499908447266</v>
@@ -7215,22 +7215,22 @@
         <v>1</v>
       </c>
       <c r="D212" t="n">
-        <v>11709.07485368447</v>
+        <v>12259.79779899607</v>
       </c>
       <c r="E212" t="n">
-        <v>17108</v>
+        <v>17915</v>
       </c>
       <c r="F212" t="n">
-        <v>1154523.461801316</v>
+        <v>1208981.784130936</v>
       </c>
       <c r="G212" t="n">
         <v>66.79999923706055</v>
       </c>
       <c r="H212" t="n">
-        <v>755.6386321685792</v>
+        <v>787.9831917991638</v>
       </c>
       <c r="I212" t="n">
-        <v>1143570.0255798</v>
+        <v>1197509.969523739</v>
       </c>
       <c r="J212" t="n">
         <v>0</v>
@@ -7247,22 +7247,22 @@
         <v>1</v>
       </c>
       <c r="D213" t="n">
-        <v>127.7440182871305</v>
+        <v>147.8287642701169</v>
       </c>
       <c r="E213" t="n">
-        <v>17282</v>
+        <v>18097</v>
       </c>
       <c r="F213" t="n">
-        <v>1145751.539840431</v>
+        <v>1199797.975332568</v>
       </c>
       <c r="G213" t="n">
         <v>66.29000091552734</v>
       </c>
       <c r="H213" t="n">
-        <v>46.87067609558106</v>
+        <v>47.18886809997559</v>
       </c>
       <c r="I213" t="n">
-        <v>1155151.356415198</v>
+        <v>1209621.938558465</v>
       </c>
       <c r="J213" t="n">
         <v>0</v>
@@ -7279,25 +7279,25 @@
         <v>-1</v>
       </c>
       <c r="D214" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="E214" t="n">
         <v>0</v>
       </c>
       <c r="F214" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="G214" t="n">
         <v>66.65000152587891</v>
       </c>
       <c r="H214" t="n">
-        <v>761.0571958221436</v>
+        <v>793.6490465682984</v>
       </c>
       <c r="I214" t="n">
         <v>0</v>
       </c>
       <c r="J214" t="n">
-        <v>-4067.087240780704</v>
+        <v>-4250.509991202503</v>
       </c>
     </row>
     <row r="215">
@@ -7311,13 +7311,13 @@
         <v>0</v>
       </c>
       <c r="D215" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="E215" t="n">
         <v>0</v>
       </c>
       <c r="F215" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="G215" t="n">
         <v>66.63999938964844</v>
@@ -7343,13 +7343,13 @@
         <v>0</v>
       </c>
       <c r="D216" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="E216" t="n">
         <v>0</v>
       </c>
       <c r="F216" t="n">
-        <v>1151212.013192704</v>
+        <v>1205519.257331532</v>
       </c>
       <c r="G216" t="n">
         <v>67.10499954223633</v>
@@ -7375,22 +7375,22 @@
         <v>1</v>
       </c>
       <c r="D217" t="n">
-        <v>11649.81556941545</v>
+        <v>12208.06001221633</v>
       </c>
       <c r="E217" t="n">
-        <v>16939</v>
+        <v>17738</v>
       </c>
       <c r="F217" t="n">
-        <v>1150458.777815357</v>
+        <v>1204733.791892404</v>
       </c>
       <c r="G217" t="n">
         <v>67.22999954223633</v>
       </c>
       <c r="H217" t="n">
-        <v>753.2353773475647</v>
+        <v>785.4654391281128</v>
       </c>
       <c r="I217" t="n">
-        <v>1139562.197623289</v>
+        <v>1193311.197319316</v>
       </c>
       <c r="J217" t="n">
         <v>0</v>
@@ -7407,13 +7407,13 @@
         <v>0</v>
       </c>
       <c r="D218" t="n">
-        <v>11649.81556941545</v>
+        <v>12208.06001221633</v>
       </c>
       <c r="E218" t="n">
-        <v>16939</v>
+        <v>17738</v>
       </c>
       <c r="F218" t="n">
-        <v>1151136.353323474</v>
+        <v>1205443.328132028</v>
       </c>
       <c r="G218" t="n">
         <v>67.27000045776367</v>
@@ -7422,7 +7422,7 @@
         <v>0</v>
       </c>
       <c r="I218" t="n">
-        <v>1139562.197623289</v>
+        <v>1193311.197319316</v>
       </c>
       <c r="J218" t="n">
         <v>0</v>
@@ -7439,25 +7439,25 @@
         <v>-1</v>
       </c>
       <c r="D219" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E219" t="n">
         <v>0</v>
       </c>
       <c r="F219" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G219" t="n">
         <v>67.83000183105469</v>
       </c>
       <c r="H219" t="n">
-        <v>759.3334406097413</v>
+        <v>791.8511434875489</v>
       </c>
       <c r="I219" t="n">
         <v>0</v>
       </c>
       <c r="J219" t="n">
-        <v>8650.869952336885</v>
+        <v>9065.524016444338</v>
       </c>
     </row>
     <row r="220">
@@ -7471,13 +7471,13 @@
         <v>0</v>
       </c>
       <c r="D220" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E220" t="n">
         <v>0</v>
       </c>
       <c r="F220" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G220" t="n">
         <v>68.61999893188477</v>
@@ -7503,13 +7503,13 @@
         <v>-1</v>
       </c>
       <c r="D221" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E221" t="n">
         <v>0</v>
       </c>
       <c r="F221" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G221" t="n">
         <v>69.05999755859375</v>
@@ -7535,13 +7535,13 @@
         <v>0</v>
       </c>
       <c r="D222" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E222" t="n">
         <v>0</v>
       </c>
       <c r="F222" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G222" t="n">
         <v>68.45499801635742</v>
@@ -7567,13 +7567,13 @@
         <v>-1</v>
       </c>
       <c r="D223" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E223" t="n">
         <v>0</v>
       </c>
       <c r="F223" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G223" t="n">
         <v>67.86999893188477</v>
@@ -7599,13 +7599,13 @@
         <v>-1</v>
       </c>
       <c r="D224" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E224" t="n">
         <v>0</v>
       </c>
       <c r="F224" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G224" t="n">
         <v>67.81000137329102</v>
@@ -7631,13 +7631,13 @@
         <v>0</v>
       </c>
       <c r="D225" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="E225" t="n">
         <v>0</v>
       </c>
       <c r="F225" t="n">
-        <v>1159862.883145041</v>
+        <v>1214584.781347977</v>
       </c>
       <c r="G225" t="n">
         <v>66.23000335693359</v>
@@ -7663,22 +7663,22 @@
         <v>1</v>
       </c>
       <c r="D226" t="n">
-        <v>11749.93387579668</v>
+        <v>12356.85819964226</v>
       </c>
       <c r="E226" t="n">
-        <v>17672</v>
+        <v>18505</v>
       </c>
       <c r="F226" t="n">
-        <v>1159104.520393131</v>
+        <v>1213793.969081448</v>
       </c>
       <c r="G226" t="n">
         <v>64.92499923706055</v>
       </c>
       <c r="H226" t="n">
-        <v>758.3627519104004</v>
+        <v>790.8122665290833</v>
       </c>
       <c r="I226" t="n">
-        <v>1148112.949269244</v>
+        <v>1202227.923148334</v>
       </c>
       <c r="J226" t="n">
         <v>0</v>
@@ -7695,22 +7695,22 @@
         <v>1</v>
       </c>
       <c r="D227" t="n">
-        <v>95.63961085832528</v>
+        <v>115.3218089485972</v>
       </c>
       <c r="E227" t="n">
-        <v>17850</v>
+        <v>18692</v>
       </c>
       <c r="F227" t="n">
-        <v>1164094.123268695</v>
+        <v>1219020.624695912</v>
       </c>
       <c r="G227" t="n">
         <v>65.20999908447266</v>
       </c>
       <c r="H227" t="n">
-        <v>46.91442790222168</v>
+        <v>47.26656189727784</v>
       </c>
       <c r="I227" t="n">
-        <v>1159767.243534183</v>
+        <v>1214469.459539028</v>
       </c>
       <c r="J227" t="n">
         <v>0</v>
@@ -7727,13 +7727,13 @@
         <v>1</v>
       </c>
       <c r="D228" t="n">
-        <v>16.50961329973153</v>
+        <v>36.19181139000344</v>
       </c>
       <c r="E228" t="n">
-        <v>17851</v>
+        <v>18693</v>
       </c>
       <c r="F228" t="n">
-        <v>1179253.526031757</v>
+        <v>1234895.726174183</v>
       </c>
       <c r="G228" t="n">
         <v>66.05999755859375</v>
@@ -7742,7 +7742,7 @@
         <v>13.07</v>
       </c>
       <c r="I228" t="n">
-        <v>1159846.373531742</v>
+        <v>1214548.589536587</v>
       </c>
       <c r="J228" t="n">
         <v>0</v>
@@ -7759,13 +7759,13 @@
         <v>1</v>
       </c>
       <c r="D229" t="n">
-        <v>16.50961329973153</v>
+        <v>36.19181139000344</v>
       </c>
       <c r="E229" t="n">
-        <v>17851</v>
+        <v>18693</v>
       </c>
       <c r="F229" t="n">
-        <v>1185947.719127918</v>
+        <v>1241905.672482319</v>
       </c>
       <c r="G229" t="n">
         <v>66.43500137329102</v>
@@ -7774,7 +7774,7 @@
         <v>0</v>
       </c>
       <c r="I229" t="n">
-        <v>1159846.373531742</v>
+        <v>1214548.589536587</v>
       </c>
       <c r="J229" t="n">
         <v>0</v>
@@ -7791,13 +7791,13 @@
         <v>1</v>
       </c>
       <c r="D230" t="n">
-        <v>16.50961329973153</v>
+        <v>36.19181139000344</v>
       </c>
       <c r="E230" t="n">
-        <v>17851</v>
+        <v>18693</v>
       </c>
       <c r="F230" t="n">
-        <v>1177736.275470996</v>
+        <v>1233306.909596272</v>
       </c>
       <c r="G230" t="n">
         <v>65.97500228881836</v>
@@ -7806,7 +7806,7 @@
         <v>0</v>
       </c>
       <c r="I230" t="n">
-        <v>1159846.373531742</v>
+        <v>1214548.589536587</v>
       </c>
       <c r="J230" t="n">
         <v>0</v>
@@ -7823,13 +7823,13 @@
         <v>1</v>
       </c>
       <c r="D231" t="n">
-        <v>16.50961329973153</v>
+        <v>36.19181139000344</v>
       </c>
       <c r="E231" t="n">
-        <v>17851</v>
+        <v>18693</v>
       </c>
       <c r="F231" t="n">
-        <v>1180770.912784839</v>
+        <v>1236484.685368366</v>
       </c>
       <c r="G231" t="n">
         <v>66.14500045776367</v>
@@ -7838,7 +7838,7 @@
         <v>0</v>
       </c>
       <c r="I231" t="n">
-        <v>1159846.373531742</v>
+        <v>1214548.589536587</v>
       </c>
       <c r="J231" t="n">
         <v>0</v>
@@ -7855,25 +7855,25 @@
         <v>-1</v>
       </c>
       <c r="D232" t="n">
-        <v>1195691.983870421</v>
+        <v>1252112.85632253</v>
       </c>
       <c r="E232" t="n">
         <v>0</v>
       </c>
       <c r="F232" t="n">
-        <v>1195691.983870421</v>
+        <v>1252112.85632253</v>
       </c>
       <c r="G232" t="n">
         <v>67.02500152587891</v>
       </c>
       <c r="H232" t="n">
-        <v>787.8279813430787</v>
+        <v>821.6890121139527</v>
       </c>
       <c r="I232" t="n">
         <v>0</v>
       </c>
       <c r="J232" t="n">
-        <v>35829.10072537977</v>
+        <v>37528.07497455366</v>
       </c>
     </row>
     <row r="233">
@@ -7887,22 +7887,22 @@
         <v>1</v>
       </c>
       <c r="D233" t="n">
-        <v>12125.39351935296</v>
+        <v>12713.44598179404</v>
       </c>
       <c r="E233" t="n">
-        <v>17848</v>
+        <v>18690</v>
       </c>
       <c r="F233" t="n">
-        <v>1194912.361689519</v>
+        <v>1251299.754537397</v>
       </c>
       <c r="G233" t="n">
         <v>66.27000045776367</v>
       </c>
       <c r="H233" t="n">
-        <v>779.6221809020997</v>
+        <v>813.1017851333619</v>
       </c>
       <c r="I233" t="n">
-        <v>1183566.590351068</v>
+        <v>1239399.410340736</v>
       </c>
       <c r="J233" t="n">
         <v>0</v>
@@ -7919,25 +7919,25 @@
         <v>-1</v>
       </c>
       <c r="D234" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E234" t="n">
         <v>0</v>
       </c>
       <c r="F234" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G234" t="n">
         <v>65.30000305175781</v>
       </c>
       <c r="H234" t="n">
-        <v>769.2346726806641</v>
+        <v>802.2242342224122</v>
       </c>
       <c r="I234" t="n">
         <v>0</v>
       </c>
       <c r="J234" t="n">
-        <v>-18861.37055597547</v>
+        <v>-19744.57753760531</v>
       </c>
     </row>
     <row r="235">
@@ -7951,13 +7951,13 @@
         <v>0</v>
       </c>
       <c r="D235" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E235" t="n">
         <v>0</v>
       </c>
       <c r="F235" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G235" t="n">
         <v>64.92500305175781</v>
@@ -7983,13 +7983,13 @@
         <v>-1</v>
       </c>
       <c r="D236" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E236" t="n">
         <v>0</v>
       </c>
       <c r="F236" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G236" t="n">
         <v>64.92000198364258</v>
@@ -8015,13 +8015,13 @@
         <v>0</v>
       </c>
       <c r="D237" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E237" t="n">
         <v>0</v>
       </c>
       <c r="F237" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G237" t="n">
         <v>65.1150016784668</v>
@@ -8047,13 +8047,13 @@
         <v>0</v>
       </c>
       <c r="D238" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E238" t="n">
         <v>0</v>
       </c>
       <c r="F238" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G238" t="n">
         <v>65.33000183105469</v>
@@ -8079,13 +8079,13 @@
         <v>-1</v>
       </c>
       <c r="D239" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E239" t="n">
         <v>0</v>
       </c>
       <c r="F239" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G239" t="n">
         <v>65.125</v>
@@ -8111,13 +8111,13 @@
         <v>-1</v>
       </c>
       <c r="D240" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E240" t="n">
         <v>0</v>
       </c>
       <c r="F240" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G240" t="n">
         <v>64.33999824523926</v>
@@ -8143,13 +8143,13 @@
         <v>0</v>
       </c>
       <c r="D241" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="E241" t="n">
         <v>0</v>
       </c>
       <c r="F241" t="n">
-        <v>1176830.613314446</v>
+        <v>1232368.278784925</v>
       </c>
       <c r="G241" t="n">
         <v>64.75499725341797</v>
@@ -8175,22 +8175,22 @@
         <v>1</v>
       </c>
       <c r="D242" t="n">
-        <v>11936.9381644456</v>
+        <v>12501.13933492512</v>
       </c>
       <c r="E242" t="n">
-        <v>17841</v>
+        <v>18683</v>
       </c>
       <c r="F242" t="n">
-        <v>1176062.188164446</v>
+        <v>1231566.889334925</v>
       </c>
       <c r="G242" t="n">
         <v>65.25</v>
       </c>
       <c r="H242" t="n">
-        <v>768.42515</v>
+        <v>801.38945</v>
       </c>
       <c r="I242" t="n">
-        <v>1164893.67515</v>
+        <v>1219867.13945</v>
       </c>
       <c r="J242" t="n">
         <v>0</v>
@@ -8207,25 +8207,25 @@
         <v>-1</v>
       </c>
       <c r="D243" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="E243" t="n">
         <v>0</v>
       </c>
       <c r="F243" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="G243" t="n">
         <v>65.84000015258789</v>
       </c>
       <c r="H243" t="n">
-        <v>774.7408656333923</v>
+        <v>808.0032337104798</v>
       </c>
       <c r="I243" t="n">
         <v>0</v>
       </c>
       <c r="J243" t="n">
-        <v>8983.026706687175</v>
+        <v>9413.580167089123</v>
       </c>
     </row>
     <row r="244">
@@ -8239,13 +8239,13 @@
         <v>-1</v>
       </c>
       <c r="D244" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="E244" t="n">
         <v>0</v>
       </c>
       <c r="F244" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="G244" t="n">
         <v>65.23500061035156</v>
@@ -8271,13 +8271,13 @@
         <v>-1</v>
       </c>
       <c r="D245" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="E245" t="n">
         <v>0</v>
       </c>
       <c r="F245" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="G245" t="n">
         <v>65.51000213623047</v>
@@ -8303,13 +8303,13 @@
         <v>-1</v>
       </c>
       <c r="D246" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="E246" t="n">
         <v>0</v>
       </c>
       <c r="F246" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="G246" t="n">
         <v>64.2599983215332</v>
@@ -8335,13 +8335,13 @@
         <v>0</v>
       </c>
       <c r="D247" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="E247" t="n">
         <v>0</v>
       </c>
       <c r="F247" t="n">
-        <v>1185813.640021133</v>
+        <v>1241781.858952014</v>
       </c>
       <c r="G247" t="n">
         <v>61.06999969482422</v>
@@ -8367,22 +8367,22 @@
         <v>1</v>
       </c>
       <c r="D248" t="n">
-        <v>12058.36827215053</v>
+        <v>12621.40342104729</v>
       </c>
       <c r="E248" t="n">
-        <v>18684</v>
+        <v>19566</v>
       </c>
       <c r="F248" t="n">
-        <v>1185039.901101435</v>
+        <v>1240974.896855953</v>
       </c>
       <c r="G248" t="n">
         <v>62.78000068664551</v>
       </c>
       <c r="H248" t="n">
-        <v>773.738919697571</v>
+        <v>806.9620960609436</v>
       </c>
       <c r="I248" t="n">
-        <v>1173755.271748982</v>
+        <v>1229160.455530967</v>
       </c>
       <c r="J248" t="n">
         <v>0</v>
@@ -8399,25 +8399,25 @@
         <v>-1</v>
       </c>
       <c r="D249" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="E249" t="n">
         <v>0</v>
       </c>
       <c r="F249" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="G249" t="n">
         <v>63.07500076293945</v>
       </c>
       <c r="H249" t="n">
-        <v>777.0459885528566</v>
+        <v>810.4252789566041</v>
       </c>
       <c r="I249" t="n">
         <v>0</v>
       </c>
       <c r="J249" t="n">
-        <v>3960.996517225634</v>
+        <v>4154.584117749939</v>
       </c>
     </row>
     <row r="250">
@@ -8431,13 +8431,13 @@
         <v>0</v>
       </c>
       <c r="D250" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="E250" t="n">
         <v>0</v>
       </c>
       <c r="F250" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="G250" t="n">
         <v>63.97500038146973</v>
@@ -8463,13 +8463,13 @@
         <v>-1</v>
       </c>
       <c r="D251" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="E251" t="n">
         <v>0</v>
       </c>
       <c r="F251" t="n">
-        <v>1189774.636538358</v>
+        <v>1245936.443069764</v>
       </c>
       <c r="G251" t="n">
         <v>63.58499908447266</v>
@@ -8495,22 +8495,22 @@
         <v>1</v>
       </c>
       <c r="D252" t="n">
-        <v>12088.97188832178</v>
+        <v>12649.06792172341</v>
       </c>
       <c r="E252" t="n">
-        <v>18172</v>
+        <v>19030</v>
       </c>
       <c r="F252" t="n">
-        <v>1188998.540797013</v>
+        <v>1245127.006306733</v>
       </c>
       <c r="G252" t="n">
         <v>64.76499938964844</v>
       </c>
       <c r="H252" t="n">
-        <v>776.0957413452148</v>
+        <v>809.436763031006</v>
       </c>
       <c r="I252" t="n">
-        <v>1177685.664650037</v>
+        <v>1233287.375148041</v>
       </c>
       <c r="J252" t="n">
         <v>0</v>
@@ -8527,25 +8527,25 @@
         <v>-1</v>
       </c>
       <c r="D253" t="n">
-        <v>1197030.588088322</v>
+        <v>1253541.593421723</v>
       </c>
       <c r="E253" t="n">
         <v>0</v>
       </c>
       <c r="F253" t="n">
-        <v>1197030.588088322</v>
+        <v>1253541.593421723</v>
       </c>
       <c r="G253" t="n">
         <v>65.25</v>
       </c>
       <c r="H253" t="n">
-        <v>781.3838000000001</v>
+        <v>814.9745</v>
       </c>
       <c r="I253" t="n">
         <v>0</v>
       </c>
       <c r="J253" t="n">
-        <v>7255.951549963327</v>
+        <v>7605.150351959281</v>
       </c>
     </row>
     <row r="254">
@@ -8559,13 +8559,13 @@
         <v>0</v>
       </c>
       <c r="D254" t="n">
-        <v>1197030.588088322</v>
+        <v>1253541.593421723</v>
       </c>
       <c r="E254" t="n">
         <v>0</v>
       </c>
       <c r="F254" t="n">
-        <v>1197030.588088322</v>
+        <v>1253541.593421723</v>
       </c>
       <c r="G254" t="n">
         <v>65.44999694824219</v>
@@ -8591,22 +8591,22 @@
         <v>1</v>
       </c>
       <c r="D255" t="n">
-        <v>12123.47241159062</v>
+        <v>12754.02341411695</v>
       </c>
       <c r="E255" t="n">
-        <v>17959</v>
+        <v>18806</v>
       </c>
       <c r="F255" t="n">
-        <v>1196250.162074524</v>
+        <v>1252727.659240228</v>
       </c>
       <c r="G255" t="n">
         <v>65.93500137329102</v>
       </c>
       <c r="H255" t="n">
-        <v>780.42601379776</v>
+        <v>813.9341814956665</v>
       </c>
       <c r="I255" t="n">
-        <v>1184907.115676731</v>
+        <v>1240787.570007606</v>
       </c>
       <c r="J255" t="n">
         <v>0</v>

</xml_diff>